<commit_message>
Inicio site do produto
</commit_message>
<xml_diff>
--- a/documentacao/Planilha de backlogs.xlsx
+++ b/documentacao/Planilha de backlogs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leticia\Documents\git PI\P.I\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ultim\Desktop\BandTec\git\P.I\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2518258B-A0C2-4699-9684-12D2474E32D3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B638F17-5E48-4C33-B496-9993B8309E46}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1395" yWindow="1080" windowWidth="16530" windowHeight="9345" activeTab="3" xr2:uid="{63126B56-C87D-495C-B963-22CEEB379DE7}"/>
+    <workbookView xWindow="1395" yWindow="1080" windowWidth="16530" windowHeight="9345" activeTab="2" xr2:uid="{63126B56-C87D-495C-B963-22CEEB379DE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Requisitos" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Project Backlog" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1673,7 +1672,7 @@
       <c r="E25" s="34"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E25">
+  <sortState ref="A2:E25">
     <sortCondition ref="E25"/>
   </sortState>
   <mergeCells count="4">
@@ -2040,8 +2039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1FB5F1F-A67C-4DD1-A12A-B74E89955FF0}">
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2293,7 +2292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5751B30-C353-40A7-AF36-A92540DAB466}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>